<commit_message>
Added some link to my excell sheet that will be useful for the Advanced Artifiial Intelligence Assignment
</commit_message>
<xml_diff>
--- a/Advanced Artificial Intelligence/AAI Assignment 1/Assignment Excell CPT.xlsx
+++ b/Advanced Artificial Intelligence/AAI Assignment 1/Assignment Excell CPT.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Computing\Desktop\MSc-Robotics-and-Autonomous-Systems\Advanced Artificial Intelligence\AAI Assignment 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ff494b0457865fe3/Desktop/MSc-Robotics-and-Autonomous-Systems/Advanced Artificial Intelligence/AAI Assignment 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_08D6C05C7192E5440E4A888A64ADC27804645A78" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F866B2A1-A3B0-4ED6-8F36-F610DE1F29F6}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="57480" yWindow="3855" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>P(Y|Z)</t>
   </si>
@@ -87,12 +88,18 @@
   </si>
   <si>
     <t>Treatment</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/55926173/compare-elements-in-dataframe-columns-for-each-row-python</t>
+  </si>
+  <si>
+    <t>https://medium.com/analytics-vidhya/comparison-of-two-data-sets-using-python-a24a6d8beb13</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -421,27 +428,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:P15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B3:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" customWidth="1"/>
+    <col min="7" max="7" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1796875" customWidth="1"/>
+    <col min="10" max="10" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1796875" customWidth="1"/>
+    <col min="14" max="14" width="12.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
@@ -479,7 +486,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="b">
         <v>1</v>
       </c>
@@ -511,7 +518,7 @@
         <v>0.17100000000000001</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="b">
         <v>0</v>
       </c>
@@ -535,7 +542,7 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
@@ -565,7 +572,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="b">
         <v>1</v>
       </c>
@@ -587,7 +594,7 @@
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="b">
         <v>0</v>
       </c>
@@ -599,7 +606,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
@@ -613,7 +620,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B12" s="1" t="s">
         <v>16</v>
       </c>
@@ -623,7 +630,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
@@ -633,7 +640,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B14" s="1" t="s">
         <v>17</v>
       </c>
@@ -643,7 +650,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B15" s="1" t="s">
         <v>17</v>
       </c>
@@ -652,6 +659,16 @@
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Working on Advanced Artificial Intelligence assignment, Almost finished CPT for all variables
</commit_message>
<xml_diff>
--- a/Advanced Artificial Intelligence/AAI Assignment 1/Assignment Excell CPT.xlsx
+++ b/Advanced Artificial Intelligence/AAI Assignment 1/Assignment Excell CPT.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ff494b0457865fe3/Desktop/MSc-Robotics-and-Autonomous-Systems/Advanced Artificial Intelligence/AAI Assignment 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Computing\Desktop\MSc-Robotics-and-Autonomous-Systems\Advanced Artificial Intelligence\AAI Assignment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_08D6C05C7192E5440E4A888A64ADC27804645A78" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F866B2A1-A3B0-4ED6-8F36-F610DE1F29F6}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="3855" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="3855" windowWidth="29040" windowHeight="15225"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t>P(Y|Z)</t>
   </si>
@@ -42,9 +41,6 @@
     <t>P(X|Z)</t>
   </si>
   <si>
-    <t>Health(Z)</t>
-  </si>
-  <si>
     <t>Z</t>
   </si>
   <si>
@@ -84,26 +80,55 @@
     <t>P(Y,X/¬Z)</t>
   </si>
   <si>
-    <t>P(¬X)</t>
-  </si>
-  <si>
-    <t>Treatment</t>
-  </si>
-  <si>
     <t>https://stackoverflow.com/questions/55926173/compare-elements-in-dataframe-columns-for-each-row-python</t>
   </si>
   <si>
     <t>https://medium.com/analytics-vidhya/comparison-of-two-data-sets-using-python-a24a6d8beb13</t>
+  </si>
+  <si>
+    <t>No treatment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medication </t>
+  </si>
+  <si>
+    <t>Placebo</t>
+  </si>
+  <si>
+    <t>Survive</t>
+  </si>
+  <si>
+    <t>Healthy</t>
+  </si>
+  <si>
+    <t>TT</t>
+  </si>
+  <si>
+    <t>FT</t>
+  </si>
+  <si>
+    <t>TF</t>
+  </si>
+  <si>
+    <t>FF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -141,16 +166,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -428,85 +456,102 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:P19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1796875" customWidth="1"/>
-    <col min="7" max="7" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1796875" customWidth="1"/>
-    <col min="10" max="10" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.1796875" customWidth="1"/>
-    <col min="14" max="14" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="b">
         <v>1</v>
       </c>
       <c r="C4" s="1">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="D4" s="1"/>
+        <v>0.09</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.91</v>
+      </c>
       <c r="F4" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="G4" s="1">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.92800000000000005</v>
+      </c>
       <c r="J4" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K4" s="1">
-        <v>0.17100000000000001</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="L4" s="1">
-        <v>0.82899999999999996</v>
+        <v>0.95699999999999996</v>
       </c>
       <c r="N4" s="1" t="b">
         <v>1</v>
@@ -518,61 +563,73 @@
         <v>0.17100000000000001</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="b">
         <v>0</v>
       </c>
       <c r="C5" s="1">
-        <v>0.71</v>
-      </c>
-      <c r="D5" s="1"/>
+        <v>0.90200000000000002</v>
+      </c>
+      <c r="D5" s="1">
+        <v>9.8000000000000004E-2</v>
+      </c>
       <c r="F5" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+      <c r="G5" s="1">
+        <v>0.90200000000000002</v>
+      </c>
+      <c r="H5" s="1">
+        <v>9.8000000000000004E-2</v>
+      </c>
       <c r="J5" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
+      <c r="K5" s="1">
+        <v>0.39</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0.61</v>
+      </c>
       <c r="N5" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I7" s="2"/>
-      <c r="J7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="b">
         <v>1</v>
       </c>
@@ -590,11 +647,11 @@
         <v>0.27200000000000002</v>
       </c>
       <c r="I8" s="2"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="b">
         <v>0</v>
       </c>
@@ -606,71 +663,87 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B12" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="C12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="G12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B19" t="s">
-        <v>22</v>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B19" r:id="rId1"/>
+    <hyperlink ref="B18" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finishing CPT tables for AI assignment
</commit_message>
<xml_diff>
--- a/Advanced Artificial Intelligence/AAI Assignment 1/Assignment Excell CPT.xlsx
+++ b/Advanced Artificial Intelligence/AAI Assignment 1/Assignment Excell CPT.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
   <si>
     <t>P(Y|Z)</t>
   </si>
@@ -65,9 +65,6 @@
     <t>P(X|¬Z)</t>
   </si>
   <si>
-    <t>P(X)</t>
-  </si>
-  <si>
     <t>T</t>
   </si>
   <si>
@@ -92,18 +89,6 @@
     <t>Healthy</t>
   </si>
   <si>
-    <t>TT</t>
-  </si>
-  <si>
-    <t>FT</t>
-  </si>
-  <si>
-    <t>TF</t>
-  </si>
-  <si>
-    <t>FF</t>
-  </si>
-  <si>
     <t>Most Healthy people don't get treatment</t>
   </si>
   <si>
@@ -114,6 +99,15 @@
   </si>
   <si>
     <t>P(Y|X,¬Z)</t>
+  </si>
+  <si>
+    <t>P(X=1)</t>
+  </si>
+  <si>
+    <t>P(X=0)</t>
+  </si>
+  <si>
+    <t>P(Z=0)</t>
   </si>
 </sst>
 </file>
@@ -145,7 +139,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -168,18 +162,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -463,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="D17:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,13 +488,13 @@
   <sheetData>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -603,13 +609,13 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" t="s">
         <v>20</v>
       </c>
-      <c r="F6" t="s">
+      <c r="J6" t="s">
         <v>21</v>
-      </c>
-      <c r="J6" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -677,116 +683,161 @@
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="H11" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="G12" t="s">
-        <v>23</v>
-      </c>
-      <c r="H12" t="s">
-        <v>25</v>
+        <v>13</v>
+      </c>
+      <c r="D12" s="1">
+        <f>((13)*K4)/171</f>
+        <v>3.2690058479532161E-3</v>
+      </c>
+      <c r="E12" s="1">
+        <f>1-D12</f>
+        <v>0.9967309941520468</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="D13" s="1">
+        <f>((116)*K4)/171</f>
+        <v>2.9169590643274852E-2</v>
+      </c>
+      <c r="E13" s="1">
+        <f>1-D13</f>
+        <v>0.97083040935672515</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="D14" s="1">
+        <f>((135*K4))/171</f>
+        <v>3.3947368421052629E-2</v>
+      </c>
+      <c r="E14" s="1">
+        <f>1-D14</f>
+        <v>0.96605263157894739</v>
+      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="D15" s="1">
+        <f>((489)*K4)/171</f>
+        <v>0.12296491228070174</v>
+      </c>
+      <c r="E15" s="1">
+        <f>1-D15</f>
+        <v>0.87703508771929828</v>
+      </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="B16" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="2"/>
+      <c r="B17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="2">
+        <f>63</f>
+        <v>63</v>
+      </c>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="4"/>
+      <c r="B18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="4"/>
+      <c r="B19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="3" t="s">
-        <v>27</v>
-      </c>
+      <c r="B22" s="3"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="B23" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B22" r:id="rId1" display="https://stackoverflow.com/questions/55926173/compare-elements-in-dataframe-columns-for-each-row-python"/>
-    <hyperlink ref="B23" r:id="rId2"/>
+    <hyperlink ref="G11" r:id="rId1" display="https://stackoverflow.com/questions/55926173/compare-elements-in-dataframe-columns-for-each-row-python"/>
+    <hyperlink ref="G12" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixing assignment code for the CPTs
</commit_message>
<xml_diff>
--- a/Advanced Artificial Intelligence/AAI Assignment 1/Assignment Excell CPT.xlsx
+++ b/Advanced Artificial Intelligence/AAI Assignment 1/Assignment Excell CPT.xlsx
@@ -469,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="D17:E20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,12 +707,11 @@
         <v>13</v>
       </c>
       <c r="D12" s="1">
-        <f>((13)*K4)/171</f>
-        <v>3.2690058479532161E-3</v>
+        <f>1-E12</f>
+        <v>4.7399463999999725E-3</v>
       </c>
       <c r="E12" s="1">
-        <f>1-D12</f>
-        <v>0.9967309941520468</v>
+        <v>0.99526005360000003</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>15</v>
@@ -727,12 +726,11 @@
         <v>14</v>
       </c>
       <c r="D13" s="1">
-        <f>((116)*K4)/171</f>
-        <v>2.9169590643274852E-2</v>
+        <v>4.229490617E-2</v>
       </c>
       <c r="E13" s="1">
         <f>1-D13</f>
-        <v>0.97083040935672515</v>
+        <v>0.95770509383000002</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -744,12 +742,11 @@
         <v>13</v>
       </c>
       <c r="D14" s="1">
-        <f>((135*K4))/171</f>
-        <v>3.3947368421052629E-2</v>
+        <v>4.9222520110000001E-2</v>
       </c>
       <c r="E14" s="1">
         <f>1-D14</f>
-        <v>0.96605263157894739</v>
+        <v>0.95077747988999994</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -761,12 +758,11 @@
         <v>14</v>
       </c>
       <c r="D15" s="1">
-        <f>((489)*K4)/171</f>
-        <v>0.12296491228070174</v>
+        <v>0.17574262730000001</v>
       </c>
       <c r="E15" s="1">
         <f>1-D15</f>
-        <v>0.87703508771929828</v>
+        <v>0.82425737269999999</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -792,10 +788,7 @@
       <c r="C17" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="2">
-        <f>63</f>
-        <v>63</v>
-      </c>
+      <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Made a powerpoint to edit CPT Diagram
</commit_message>
<xml_diff>
--- a/Advanced Artificial Intelligence/AAI Assignment 1/Assignment Excell CPT.xlsx
+++ b/Advanced Artificial Intelligence/AAI Assignment 1/Assignment Excell CPT.xlsx
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="29">
-  <si>
-    <t>P(Y|Z)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="21">
   <si>
     <t>P(x2/X|Z)</t>
   </si>
@@ -38,21 +35,9 @@
     <t>P(x0/X|Z)</t>
   </si>
   <si>
-    <t>P(X|Z)</t>
-  </si>
-  <si>
     <t>Z</t>
   </si>
   <si>
-    <t>P(Z)</t>
-  </si>
-  <si>
-    <t>P(¬Z)</t>
-  </si>
-  <si>
-    <t>P(Y|¬Z)</t>
-  </si>
-  <si>
     <t>P(x2/X|¬Z)</t>
   </si>
   <si>
@@ -62,9 +47,6 @@
     <t>P(x0/X|¬Z)</t>
   </si>
   <si>
-    <t>P(X|¬Z)</t>
-  </si>
-  <si>
     <t>T</t>
   </si>
   <si>
@@ -81,12 +63,6 @@
   </si>
   <si>
     <t>Placebo</t>
-  </si>
-  <si>
-    <t>Survive</t>
-  </si>
-  <si>
-    <t>Healthy</t>
   </si>
   <si>
     <t>Most Healthy people don't get treatment</t>
@@ -462,8 +438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,52 +457,49 @@
   <sheetData>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="J2" t="s">
-        <v>16</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="J3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="L3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>12</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="b">
@@ -556,15 +529,9 @@
       <c r="L4" s="1">
         <v>0.95699999999999996</v>
       </c>
-      <c r="N4" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="O4" s="1">
-        <v>0.82899999999999996</v>
-      </c>
-      <c r="P4" s="1">
-        <v>0.17100000000000001</v>
-      </c>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="b">
@@ -594,81 +561,46 @@
       <c r="L5" s="1">
         <v>0.61</v>
       </c>
-      <c r="N5" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" t="s">
-        <v>20</v>
-      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
       <c r="J6" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0.58399999999999996</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0.41599999999999998</v>
-      </c>
-      <c r="F8" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0.72799999999999998</v>
-      </c>
-      <c r="H8" s="1">
-        <v>0.27200000000000002</v>
-      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0.86699999999999999</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0.13300000000000001</v>
-      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -676,28 +608,28 @@
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D12" s="1">
         <f>1-E12</f>
@@ -707,16 +639,16 @@
         <v>0.99526005360000003</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D13" s="1">
         <v>4.229490617E-2</v>
@@ -729,10 +661,10 @@
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D14" s="1">
         <v>4.9222520110000001E-2</v>
@@ -745,10 +677,10 @@
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D15" s="1">
         <v>0.17574262730000001</v>
@@ -761,25 +693,25 @@
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="5" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D17" s="5">
         <v>2.297050938E-2</v>
@@ -792,10 +724,10 @@
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="6" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D18" s="5">
         <v>8.8600536189999995E-2</v>
@@ -808,10 +740,10 @@
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="6" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D19" s="5">
         <v>3.0991957099999998E-2</v>
@@ -823,10 +755,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D20" s="5">
         <v>0.1294369973</v>
@@ -838,24 +770,24 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D22" s="1">
         <v>2.625201072E-2</v>
@@ -867,10 +799,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D23" s="1">
         <v>8.7142091150000003E-2</v>
@@ -882,10 +814,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" s="7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D24" s="1">
         <v>2.7710455759999999E-2</v>
@@ -897,10 +829,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D25" s="1">
         <v>0.13089544240000001</v>

</xml_diff>

<commit_message>
Working on assignment part b now
</commit_message>
<xml_diff>
--- a/Advanced Artificial Intelligence/AAI Assignment 1/Assignment Excell CPT.xlsx
+++ b/Advanced Artificial Intelligence/AAI Assignment 1/Assignment Excell CPT.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="19">
   <si>
     <t>P(x2/X|Z)</t>
   </si>
@@ -32,21 +32,12 @@
     <t>P(x1/X|Z)</t>
   </si>
   <si>
-    <t>P(x0/X|Z)</t>
-  </si>
-  <si>
     <t>Z</t>
   </si>
   <si>
     <t>P(x2/X|¬Z)</t>
   </si>
   <si>
-    <t>P(x1/X|¬Z)</t>
-  </si>
-  <si>
-    <t>P(x0/X|¬Z)</t>
-  </si>
-  <si>
     <t>T</t>
   </si>
   <si>
@@ -59,9 +50,6 @@
     <t>No treatment</t>
   </si>
   <si>
-    <t xml:space="preserve">Medication </t>
-  </si>
-  <si>
     <t>Placebo</t>
   </si>
   <si>
@@ -87,6 +75,12 @@
   </si>
   <si>
     <t>P(X=2)</t>
+  </si>
+  <si>
+    <t>P(x0|Z)</t>
+  </si>
+  <si>
+    <t>Medicine</t>
   </si>
 </sst>
 </file>
@@ -439,7 +433,7 @@
   <dimension ref="A2:P25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,13 +451,13 @@
   <sheetData>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="J2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
@@ -471,32 +465,28 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="H3" s="1"/>
       <c r="J3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="L3" s="1"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
@@ -515,20 +505,16 @@
         <v>1</v>
       </c>
       <c r="G4" s="1">
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0.92800000000000005</v>
-      </c>
+        <v>0.49</v>
+      </c>
+      <c r="H4" s="1"/>
       <c r="J4" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K4" s="1">
-        <v>4.2999999999999997E-2</v>
-      </c>
-      <c r="L4" s="1">
-        <v>0.95699999999999996</v>
-      </c>
+        <v>0.61</v>
+      </c>
+      <c r="L4" s="1"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
@@ -547,20 +533,16 @@
         <v>0</v>
       </c>
       <c r="G5" s="1">
-        <v>0.90200000000000002</v>
-      </c>
-      <c r="H5" s="1">
-        <v>9.8000000000000004E-2</v>
-      </c>
+        <v>0.08</v>
+      </c>
+      <c r="H5" s="1"/>
       <c r="J5" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K5" s="1">
-        <v>0.39</v>
-      </c>
-      <c r="L5" s="1">
-        <v>0.61</v>
-      </c>
+        <v>0.04</v>
+      </c>
+      <c r="L5" s="1"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
@@ -570,7 +552,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="J6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -608,28 +590,28 @@
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D12" s="1">
         <f>1-E12</f>
@@ -639,16 +621,16 @@
         <v>0.99526005360000003</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D13" s="1">
         <v>4.229490617E-2</v>
@@ -661,10 +643,10 @@
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D14" s="1">
         <v>4.9222520110000001E-2</v>
@@ -677,10 +659,10 @@
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D15" s="1">
         <v>0.17574262730000001</v>
@@ -693,25 +675,25 @@
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D17" s="5">
         <v>2.297050938E-2</v>
@@ -724,10 +706,10 @@
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D18" s="5">
         <v>8.8600536189999995E-2</v>
@@ -740,10 +722,10 @@
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D19" s="5">
         <v>3.0991957099999998E-2</v>
@@ -755,10 +737,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D20" s="5">
         <v>0.1294369973</v>
@@ -770,24 +752,24 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D22" s="1">
         <v>2.625201072E-2</v>
@@ -799,10 +781,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D23" s="1">
         <v>8.7142091150000003E-2</v>
@@ -814,10 +796,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" s="7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D24" s="1">
         <v>2.7710455759999999E-2</v>
@@ -829,10 +811,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D25" s="1">
         <v>0.13089544240000001</v>

</xml_diff>

<commit_message>
Finished part c of assignment
</commit_message>
<xml_diff>
--- a/Advanced Artificial Intelligence/AAI Assignment 1/Assignment Excell CPT.xlsx
+++ b/Advanced Artificial Intelligence/AAI Assignment 1/Assignment Excell CPT.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Computing\Desktop\MSc-Robotics-and-Autonomous-Systems\Advanced Artificial Intelligence\AAI Assignment 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\MSc-Robotics-and-Autonomous-Systems\Advanced Artificial Intelligence\AAI Assignment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -433,7 +433,7 @@
   <dimension ref="A2:P25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,6 +499,7 @@
         <v>0.09</v>
       </c>
       <c r="D4" s="1">
+        <f>1-C4</f>
         <v>0.91</v>
       </c>
       <c r="F4" s="1" t="b">
@@ -507,14 +508,20 @@
       <c r="G4" s="1">
         <v>0.49</v>
       </c>
-      <c r="H4" s="1"/>
+      <c r="H4" s="1">
+        <f>1-G4</f>
+        <v>0.51</v>
+      </c>
       <c r="J4" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K4" s="1">
         <v>0.61</v>
       </c>
-      <c r="L4" s="1"/>
+      <c r="L4" s="1">
+        <f>1-K4</f>
+        <v>0.39</v>
+      </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
@@ -527,7 +534,8 @@
         <v>0.90200000000000002</v>
       </c>
       <c r="D5" s="1">
-        <v>9.8000000000000004E-2</v>
+        <f>1-C5</f>
+        <v>9.7999999999999976E-2</v>
       </c>
       <c r="F5" s="1" t="b">
         <v>0</v>
@@ -535,14 +543,20 @@
       <c r="G5" s="1">
         <v>0.08</v>
       </c>
-      <c r="H5" s="1"/>
+      <c r="H5" s="1">
+        <f>1-G5</f>
+        <v>0.92</v>
+      </c>
       <c r="J5" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K5" s="1">
         <v>0.04</v>
       </c>
-      <c r="L5" s="1"/>
+      <c r="L5" s="1">
+        <f>1-K5</f>
+        <v>0.96</v>
+      </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
@@ -614,11 +628,11 @@
         <v>4</v>
       </c>
       <c r="D12" s="1">
-        <f>1-E12</f>
-        <v>4.7399463999999725E-3</v>
+        <v>0.13</v>
       </c>
       <c r="E12" s="1">
-        <v>0.99526005360000003</v>
+        <f>1-D12</f>
+        <v>0.87</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>6</v>
@@ -633,11 +647,11 @@
         <v>5</v>
       </c>
       <c r="D13" s="1">
-        <v>4.229490617E-2</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="E13" s="1">
         <f>1-D13</f>
-        <v>0.95770509383000002</v>
+        <v>0.42000000000000004</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -649,11 +663,11 @@
         <v>4</v>
       </c>
       <c r="D14" s="1">
-        <v>4.9222520110000001E-2</v>
+        <v>0.15</v>
       </c>
       <c r="E14" s="1">
         <f>1-D14</f>
-        <v>0.95077747988999994</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -665,11 +679,11 @@
         <v>5</v>
       </c>
       <c r="D15" s="1">
-        <v>0.17574262730000001</v>
+        <v>0.6</v>
       </c>
       <c r="E15" s="1">
         <f>1-D15</f>
-        <v>0.82425737269999999</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -696,11 +710,11 @@
         <v>4</v>
       </c>
       <c r="D17" s="5">
-        <v>2.297050938E-2</v>
+        <v>0.15</v>
       </c>
       <c r="E17" s="1">
         <f>1-D17</f>
-        <v>0.97702949062</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -712,11 +726,11 @@
         <v>5</v>
       </c>
       <c r="D18" s="5">
-        <v>8.8600536189999995E-2</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E18" s="5">
         <f>1-D18</f>
-        <v>0.91139946381000003</v>
+        <v>0.44999999999999996</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -728,11 +742,11 @@
         <v>4</v>
       </c>
       <c r="D19" s="5">
-        <v>3.0991957099999998E-2</v>
+        <v>0.15</v>
       </c>
       <c r="E19" s="5">
         <f>1-D19</f>
-        <v>0.96900804289999998</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -743,11 +757,11 @@
         <v>5</v>
       </c>
       <c r="D20" s="5">
-        <v>0.1294369973</v>
+        <v>0.63</v>
       </c>
       <c r="E20" s="5">
         <f>1-D20</f>
-        <v>0.87056300269999998</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -772,11 +786,11 @@
         <v>4</v>
       </c>
       <c r="D22" s="1">
-        <v>2.625201072E-2</v>
+        <v>0.15</v>
       </c>
       <c r="E22" s="1">
         <f>1-D22</f>
-        <v>0.97374798927999995</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -787,11 +801,11 @@
         <v>5</v>
       </c>
       <c r="D23" s="1">
-        <v>8.7142091150000003E-2</v>
+        <v>0.66</v>
       </c>
       <c r="E23" s="1">
         <f>1-D23</f>
-        <v>0.91285790884999995</v>
+        <v>0.33999999999999997</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -802,11 +816,11 @@
         <v>4</v>
       </c>
       <c r="D24" s="1">
-        <v>2.7710455759999999E-2</v>
+        <v>0.15</v>
       </c>
       <c r="E24" s="1">
         <f>1-D24</f>
-        <v>0.97228954424000003</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -817,11 +831,11 @@
         <v>5</v>
       </c>
       <c r="D25" s="1">
-        <v>0.13089544240000001</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="E25" s="1">
         <f>1-D25</f>
-        <v>0.86910455760000005</v>
+        <v>0.43999999999999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Found out my part c of the Advanced Artificial Intelligence assignment could be wrong because conditional probabilities do not add up to 1
</commit_message>
<xml_diff>
--- a/Advanced Artificial Intelligence/AAI Assignment 1/Assignment Excell CPT.xlsx
+++ b/Advanced Artificial Intelligence/AAI Assignment 1/Assignment Excell CPT.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\MSc-Robotics-and-Autonomous-Systems\Advanced Artificial Intelligence\AAI Assignment 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Computing\Desktop\MSc-Robotics-and-Autonomous-Systems\Advanced Artificial Intelligence\AAI Assignment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,13 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="19">
-  <si>
-    <t>P(x2/X|Z)</t>
-  </si>
-  <si>
-    <t>P(x1/X|Z)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="20">
   <si>
     <t>Z</t>
   </si>
@@ -68,9 +62,6 @@
     <t>P(X=1)</t>
   </si>
   <si>
-    <t>P(X=0)</t>
-  </si>
-  <si>
     <t>P(Z=0)</t>
   </si>
   <si>
@@ -81,6 +72,18 @@
   </si>
   <si>
     <t>Medicine</t>
+  </si>
+  <si>
+    <t>P(x2|Z)</t>
+  </si>
+  <si>
+    <t>P(x1|Z)</t>
+  </si>
+  <si>
+    <t>Z=0</t>
+  </si>
+  <si>
+    <t>X=0</t>
   </si>
 </sst>
 </file>
@@ -433,7 +436,7 @@
   <dimension ref="A2:P25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,13 +454,13 @@
   <sheetData>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
@@ -465,26 +468,26 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="H3" s="1"/>
       <c r="J3" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="L3" s="1"/>
       <c r="N3" s="2"/>
@@ -566,7 +569,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="J6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -604,28 +607,28 @@
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D12" s="1">
         <v>0.13</v>
@@ -635,16 +638,16 @@
         <v>0.87</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D13" s="1">
         <v>0.57999999999999996</v>
@@ -657,10 +660,10 @@
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D14" s="1">
         <v>0.15</v>
@@ -673,10 +676,10 @@
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D15" s="1">
         <v>0.6</v>
@@ -689,25 +692,25 @@
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D17" s="5">
         <v>0.15</v>
@@ -720,10 +723,10 @@
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D18" s="5">
         <v>0.55000000000000004</v>
@@ -736,10 +739,10 @@
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D19" s="5">
         <v>0.15</v>
@@ -751,10 +754,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D20" s="5">
         <v>0.63</v>
@@ -766,24 +769,24 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D22" s="1">
         <v>0.15</v>
@@ -795,10 +798,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D23" s="1">
         <v>0.66</v>
@@ -810,10 +813,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" s="7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D24" s="1">
         <v>0.15</v>
@@ -825,10 +828,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D25" s="1">
         <v>0.56000000000000005</v>

</xml_diff>